<commit_message>
Corrected a few typos in files. Updated to display questions and save the answers.
</commit_message>
<xml_diff>
--- a/Files/Calibrated Estimator Workbook.xlsx
+++ b/Files/Calibrated Estimator Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data SS2/Python Projects/Calibrated Estimator Workshop/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED396DE-5676-F549-8EA2-29F284D0E03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5B9DF-D0A5-2645-9A51-D835C9796379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="6340" windowWidth="29040" windowHeight="14900" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
+    <workbookView xWindow="10920" yWindow="6920" windowWidth="29040" windowHeight="14900" activeTab="1" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupQuiz1" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="110">
   <si>
     <t>Question</t>
   </si>
@@ -72,9 +72,6 @@
     <t>How many poinds did the first edition of "How to Measure Anything" weigh?</t>
   </si>
   <si>
-    <t>The TV show Gilligan's Island first aired on what date?</t>
-  </si>
-  <si>
     <t>Statement</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Binary</t>
   </si>
   <si>
@@ -367,6 +361,15 @@
   </si>
   <si>
     <t>In 2014, on average, what percentage of a software development project's effort was spent in design (waterfall)?</t>
+  </si>
+  <si>
+    <t>The TV show Gilligan's Island first aired in what year?</t>
+  </si>
+  <si>
+    <t>How many inches long is a typical business card?</t>
+  </si>
+  <si>
+    <t>How many pounds did the first edition of "How to Measure Anything" weigh?</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -447,9 +450,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -771,7 +771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5982B91A-728C-224C-92C2-41F9148DB0B2}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -785,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -796,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -807,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -818,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -829,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -840,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -851,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -862,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -873,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -884,7 +886,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -892,21 +894,21 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="7">
-        <v>23646</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1964</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -914,10 +916,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -925,10 +927,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -936,10 +938,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -947,10 +949,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -958,10 +960,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -969,10 +971,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -980,10 +982,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -991,10 +993,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -1002,10 +1004,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1020,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7803A0FF-AC83-4502-83D9-7BEBECCFB4D5}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1047,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -1058,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -1066,10 +1068,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -1080,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -1091,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -1102,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -1113,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -1124,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -1132,10 +1134,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -1143,13 +1145,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="7">
-        <v>23646</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1964</v>
       </c>
     </row>
   </sheetData>
@@ -1178,18 +1180,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>726</v>
@@ -1197,10 +1199,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>3.1875</v>
@@ -1208,21 +1210,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="8">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
         <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3">
         <v>1935</v>
@@ -1230,21 +1232,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7">
         <v>0.21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>30</v>
@@ -1252,10 +1254,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <v>25</v>
@@ -1263,10 +1265,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <v>1450</v>
@@ -1274,10 +1276,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <v>0.26700000000000002</v>
@@ -1285,10 +1287,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>5.5</v>
@@ -1296,10 +1298,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3">
         <v>1458</v>
@@ -1307,10 +1309,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3">
         <v>4160</v>
@@ -1318,10 +1320,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3">
         <v>1636</v>
@@ -1329,10 +1331,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3">
         <v>196</v>
@@ -1340,10 +1342,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>6000</v>
@@ -1351,10 +1353,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3">
         <v>39</v>
@@ -1362,10 +1364,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>122</v>
@@ -1373,10 +1375,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3">
         <v>1870</v>
@@ -1384,10 +1386,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -1395,10 +1397,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="3">
         <v>50000</v>
@@ -1426,21 +1428,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3">
         <v>1976</v>
@@ -1448,10 +1450,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>26</v>
@@ -1459,10 +1461,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3">
         <v>443</v>
@@ -1470,10 +1472,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>6.9</v>
@@ -1481,21 +1483,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>135000</v>
@@ -1503,10 +1505,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <v>803</v>
@@ -1514,10 +1516,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>2394</v>
@@ -1525,10 +1527,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>200</v>
@@ -1536,10 +1538,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3">
         <v>1953</v>
@@ -1547,10 +1549,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3">
         <v>53.3</v>
@@ -1558,21 +1560,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="8">
+        <v>24</v>
+      </c>
+      <c r="C13" s="7">
         <v>0.7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>120</v>
@@ -1580,10 +1582,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3">
         <v>760</v>
@@ -1591,10 +1593,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>27</v>
@@ -1602,10 +1604,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3">
         <v>3300</v>
@@ -1613,10 +1615,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>185</v>
@@ -1624,10 +1626,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3">
         <v>1905</v>
@@ -1635,10 +1637,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3">
         <v>3212</v>
@@ -1646,10 +1648,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="3">
         <v>2.5</v>
@@ -1678,21 +1680,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -1700,10 +1702,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -1711,10 +1713,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -1722,10 +1724,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1733,10 +1735,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -1744,10 +1746,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -1755,10 +1757,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -1766,10 +1768,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1777,10 +1779,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -1788,10 +1790,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -1820,21 +1822,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -1842,10 +1844,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
@@ -1853,10 +1855,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>0</v>
@@ -1864,10 +1866,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1875,10 +1877,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -1886,10 +1888,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>0</v>
@@ -1897,10 +1899,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -1908,10 +1910,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1919,10 +1921,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -1930,10 +1932,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -1941,10 +1943,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -1952,10 +1954,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -1963,10 +1965,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>0</v>
@@ -1974,10 +1976,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -1985,10 +1987,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>0</v>
@@ -1996,10 +1998,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -2007,10 +2009,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -2018,10 +2020,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>0</v>
@@ -2029,10 +2031,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -2040,10 +2042,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -2072,21 +2074,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -2094,10 +2096,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -2105,10 +2107,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -2116,10 +2118,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -2127,10 +2129,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>0</v>
@@ -2138,10 +2140,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -2149,10 +2151,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -2160,10 +2162,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -2171,10 +2173,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -2182,10 +2184,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -2193,10 +2195,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -2204,10 +2206,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -2215,10 +2217,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -2226,10 +2228,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -2237,10 +2239,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -2248,10 +2250,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -2259,10 +2261,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -2270,10 +2272,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -2281,10 +2283,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -2292,10 +2294,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added README and requirements files. Finished basic test taking and storing within df in session_state.
</commit_message>
<xml_diff>
--- a/Files/Calibrated Estimator Workbook.xlsx
+++ b/Files/Calibrated Estimator Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data SS2/Python Projects/Calibrated Estimator Workshop/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E5B9DF-D0A5-2645-9A51-D835C9796379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9574A4C4-DB02-7A41-9857-8E36D72851C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="6920" windowWidth="29040" windowHeight="14900" activeTab="1" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
+    <workbookView xWindow="9340" yWindow="6640" windowWidth="29040" windowHeight="14900" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupQuiz1" sheetId="7" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>A kilogram is more than a pound.</t>
   </si>
   <si>
-    <t>CorrectAnswer</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>How many pounds did the first edition of "How to Measure Anything" weigh?</t>
+  </si>
+  <si>
+    <t>Solution</t>
   </si>
 </sst>
 </file>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5982B91A-728C-224C-92C2-41F9148DB0B2}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -787,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -820,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -842,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -853,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -875,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -886,7 +886,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>1964</v>
@@ -908,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -941,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -952,7 +952,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -963,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -974,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -1007,7 +1007,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7803A0FF-AC83-4502-83D9-7BEBECCFB4D5}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1038,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -1060,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -1093,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -1104,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -1115,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -1126,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>1964</v>
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1180,18 +1180,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>726</v>
@@ -1199,10 +1199,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>3.1875</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7">
         <v>0.65</v>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>1935</v>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7">
         <v>0.21</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>30</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
         <v>25</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>1450</v>
@@ -1276,10 +1276,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
         <v>0.26700000000000002</v>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>5.5</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
         <v>1458</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
         <v>4160</v>
@@ -1320,10 +1320,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>1636</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>196</v>
@@ -1342,10 +1342,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>6000</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3">
         <v>39</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
         <v>122</v>
@@ -1375,10 +1375,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3">
         <v>1870</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3">
         <v>50000</v>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1431,18 +1431,18 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>1976</v>
@@ -1450,10 +1450,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>26</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>443</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>6.9</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7">
         <v>0.2</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>135000</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
         <v>803</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>2394</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>200</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>1953</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
         <v>53.3</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
         <v>0.7</v>
@@ -1571,10 +1571,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
         <v>120</v>
@@ -1582,10 +1582,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>760</v>
@@ -1593,10 +1593,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>27</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3">
         <v>3300</v>
@@ -1615,10 +1615,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
         <v>185</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3">
         <v>1905</v>
@@ -1637,10 +1637,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3">
         <v>3212</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3">
         <v>2.5</v>
@@ -1668,7 +1668,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1683,10 +1683,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1694,7 +1694,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -1705,7 +1705,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -1716,7 +1716,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -1727,7 +1727,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1738,7 +1738,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -1749,7 +1749,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -1760,7 +1760,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1782,7 +1782,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -1793,7 +1793,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -1810,7 +1810,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1825,18 +1825,18 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>0</v>
@@ -1866,10 +1866,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -1888,10 +1888,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>0</v>
@@ -1899,10 +1899,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1921,10 +1921,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -1932,10 +1932,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -1943,10 +1943,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>0</v>
@@ -1976,10 +1976,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -1987,10 +1987,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>0</v>
@@ -1998,10 +1998,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -2009,10 +2009,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>0</v>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -2042,10 +2042,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -2062,7 +2062,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2077,18 +2077,18 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -2096,10 +2096,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -2107,10 +2107,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -2118,10 +2118,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -2129,10 +2129,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>0</v>
@@ -2140,10 +2140,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -2184,10 +2184,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -2195,10 +2195,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -2217,10 +2217,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -2228,10 +2228,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -2239,10 +2239,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -2250,10 +2250,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -2272,10 +2272,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added more quizzes. Added calculation and display of results once quiz is over.
</commit_message>
<xml_diff>
--- a/Files/Calibrated Estimator Workbook.xlsx
+++ b/Files/Calibrated Estimator Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data SS2/Python Projects/Calibrated Estimator Workshop/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9574A4C4-DB02-7A41-9857-8E36D72851C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE5FCFC-4F38-4545-9722-A72AFD385C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9340" yWindow="6640" windowWidth="29040" windowHeight="14900" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
+    <workbookView xWindow="9340" yWindow="6640" windowWidth="29040" windowHeight="14900" activeTab="4" xr2:uid="{831229E5-5C01-405D-AAA4-1BFCD7EBABBB}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupQuiz1" sheetId="7" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>A gallon of oil weighs less than a gallon of water.</t>
   </si>
   <si>
-    <t>Marks is always farther away from Earth than Venus.</t>
-  </si>
-  <si>
     <t>The Boston Red Sox won the first World Series.</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>Solution</t>
+  </si>
+  <si>
+    <t>Mars is always farther away from Earth than Venus.</t>
   </si>
 </sst>
 </file>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5982B91A-728C-224C-92C2-41F9148DB0B2}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -787,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -820,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -842,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -853,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -875,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -886,7 +886,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -894,10 +894,10 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>1964</v>
@@ -908,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -949,10 +949,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -982,10 +982,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -993,10 +993,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -1004,10 +1004,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1038,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
         <v>126</v>
@@ -1060,7 +1060,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>1685</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>3.5</v>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1969</v>
@@ -1093,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>1564</v>
@@ -1104,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>2451</v>
@@ -1115,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6">
         <v>0.78500000000000003</v>
@@ -1126,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>88</v>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>1.23</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>1964</v>
@@ -1180,18 +1180,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
         <v>726</v>
@@ -1199,10 +1199,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>3.1875</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7">
         <v>0.65</v>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1935</v>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7">
         <v>0.21</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>30</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
         <v>25</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>1450</v>
@@ -1276,10 +1276,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6">
         <v>0.26700000000000002</v>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
         <v>5.5</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
         <v>1458</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
         <v>4160</v>
@@ -1320,10 +1320,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
         <v>1636</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
         <v>196</v>
@@ -1342,10 +1342,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
         <v>6000</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
         <v>39</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>122</v>
@@ -1375,10 +1375,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3">
         <v>1870</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>50000</v>
@@ -1431,18 +1431,18 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>1976</v>
@@ -1450,10 +1450,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>26</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>443</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
         <v>6.9</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7">
         <v>0.2</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>135000</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
         <v>803</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>2394</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>200</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>1953</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3">
         <v>53.3</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="7">
         <v>0.7</v>
@@ -1571,10 +1571,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
         <v>120</v>
@@ -1582,10 +1582,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
         <v>760</v>
@@ -1593,10 +1593,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
         <v>27</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
         <v>3300</v>
@@ -1615,10 +1615,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>185</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3">
         <v>1905</v>
@@ -1637,10 +1637,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>3212</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>2.5</v>
@@ -1667,8 +1667,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA09596-10E2-44C0-9ED8-7C81399675E7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="80.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="204" verticalDpi="196" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7005C8-01D0-4D4A-A458-1735963A3A13}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1680,21 +1820,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -1702,32 +1842,32 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1735,10 +1875,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -1746,32 +1886,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1779,10 +1919,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -1790,12 +1930,122 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1805,12 +2055,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7005C8-01D0-4D4A-A458-1735963A3A13}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5231370B-85EB-FD4E-BFED-AE6D7CBA47FD}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1822,54 +2072,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -1877,43 +2127,43 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -1921,21 +2171,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -1943,10 +2193,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -1954,10 +2204,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -1965,43 +2215,43 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -2009,295 +2259,43 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="204" verticalDpi="196" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5231370B-85EB-FD4E-BFED-AE6D7CBA47FD}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="80.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>

</xml_diff>